<commit_message>
update result 20201125 & update plan 20201127
</commit_message>
<xml_diff>
--- a/20201125.xlsx
+++ b/20201125.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F348F30-0D3A-4881-945B-5D07A4CC5AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A64FCF-F821-4C7F-86E0-37D1759AD575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>일</t>
   </si>
@@ -215,6 +215,32 @@
   </si>
   <si>
     <t>F7작업</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 모빌리티
+ - DHCP 재연결 로직 구현 
+  -&gt; 기존 LAN케이블 연결되지 않은 상태로 booting된 후, DHCP시퀀스가 넘어갈 경우 그 이후에
+      DHCP를 시도하지 않던 로직을 DHCP가 완료되지 않으면, 주기적으로 DHCP시도 하도록 변경
+  - wiznet에 메일전송
+   -&gt; DHCP사용 시 Timeout적용관련 테스트 결과 전달
+    =&gt; DHCP사용 시, 비사용 시 각 3분테스트에 대한 wiresharck캡쳐 완료
+     ==&gt; 초기 부팅 시에만 27초 걸리고, 한번 끊어지면 2초내에 재연결 시도함
+   - 대역대가 다른 곳으로의 연결
+    -&gt; DHCP사용, 비사용의 여부와 상관없이 케이블이 연결된 경우 모든연결시도에 27초
+    -&gt; 케이블 단선의 경우 2초</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>출장</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>늦잠</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>출장스트레스</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -388,7 +414,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,8 +631,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -736,6 +786,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -871,7 +983,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -902,30 +1014,6 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -935,20 +1023,65 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1483,7 +1616,7 @@
   <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D3:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1537,18 +1670,22 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="25" t="s">
+      <c r="D3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>45</v>
       </c>
       <c r="H3" s="8"/>
@@ -1563,12 +1700,12 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="24"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>11</v>
@@ -1578,12 +1715,12 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="24"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="15"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>12</v>
@@ -1593,12 +1730,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="24"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="15"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>10</v>
@@ -1608,12 +1745,12 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="15"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>8</v>
@@ -1627,12 +1764,12 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>4</v>
@@ -1645,90 +1782,92 @@
       <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="15"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="G15" s="16"/>
       <c r="H15" s="8"/>
     </row>
@@ -1736,119 +1875,122 @@
       <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="17"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="17"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="17"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="17"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="17"/>
+      <c r="D20" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="17"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="17"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="17"/>
+      <c r="D23" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="G3:G14"/>
-    <mergeCell ref="G15:G23"/>
     <mergeCell ref="E3:E23"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="F3:F14"/>
-    <mergeCell ref="F15:F23"/>
+    <mergeCell ref="F15:G23"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>